<commit_message>
Updated OVW demo sheet for Architechture pages
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVMDemo_architecture.xlsx
+++ b/docs/OVW Sheets/OVMDemo_architecture.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbasta\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9735" firstSheet="35" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="en_au" sheetId="1" r:id="rId1"/>
@@ -61,7 +56,7 @@
     <sheet name="ja_jp" sheetId="40" r:id="rId47"/>
     <sheet name="uk_ua" sheetId="51" r:id="rId48"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="143">
   <si>
     <t>solutions</t>
   </si>
@@ -491,6 +486,15 @@
   </si>
   <si>
     <t>collaboration-architecture-var4</t>
+  </si>
+  <si>
+    <t>architecture-var1</t>
+  </si>
+  <si>
+    <t>architecture-var3</t>
+  </si>
+  <si>
+    <t>architecture-var4</t>
   </si>
 </sst>
 </file>
@@ -638,7 +642,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -673,7 +677,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -850,7 +854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -860,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -893,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -907,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -929,7 +933,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -961,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -975,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1014,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1028,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1042,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1081,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1095,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1133,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1147,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1161,7 +1165,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1200,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1214,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1228,7 +1232,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1267,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1281,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1295,7 +1299,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1334,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1348,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1362,7 +1366,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1401,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1415,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1429,7 +1433,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1468,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1482,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1520,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1534,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1548,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1569,7 +1573,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1601,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1615,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1654,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1668,7 +1672,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1706,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1720,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1734,7 +1738,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1773,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1787,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1801,7 +1805,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1840,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1854,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1892,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1906,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1920,7 +1924,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1941,7 +1945,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1973,7 +1977,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2011,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2025,7 +2029,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2039,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2078,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2092,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2106,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2145,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2159,7 +2163,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2173,7 +2177,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2212,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2226,7 +2230,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2240,7 +2244,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2261,7 +2265,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2293,7 +2297,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2307,7 +2311,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2346,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2360,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2374,7 +2378,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2413,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2427,7 +2431,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2441,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2480,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2494,7 +2498,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2508,7 +2512,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2547,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2561,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2575,7 +2579,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2614,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2628,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2642,7 +2646,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2681,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2695,7 +2699,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2709,7 +2713,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2730,7 +2734,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2762,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2800,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2814,7 +2818,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2828,7 +2832,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2867,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2881,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2895,7 +2899,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2916,7 +2920,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,7 +2938,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2948,7 +2952,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2962,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2983,7 +2987,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3001,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3015,7 +3019,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3029,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3068,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3082,7 +3086,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3096,7 +3100,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3135,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3149,7 +3153,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3163,7 +3167,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3202,7 +3206,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3216,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3230,7 +3234,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3251,7 +3255,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3283,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3388,7 +3392,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3402,7 +3406,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3416,7 +3420,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3437,7 +3441,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3455,7 +3459,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3469,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3489,7 +3493,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3507,7 +3511,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3521,7 +3525,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3540,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3559,7 +3563,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3573,7 +3577,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3611,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3625,7 +3629,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3639,7 +3643,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3678,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3692,7 +3696,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3712,7 +3716,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3730,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3744,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3758,7 +3762,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3797,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3811,7 +3815,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3825,7 +3829,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3864,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3878,7 +3882,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3892,7 +3896,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>

</xml_diff>